<commit_message>
Added enable option for simulation control in all projects Added link from web client to publishing server for refresh/reload
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="tiler" sheetId="4" r:id="rId4"/>
     <sheet name="Old" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="137">
   <si>
     <t>todo</t>
   </si>
@@ -428,12 +428,18 @@
   </si>
   <si>
     <t>switch to issues on github</t>
+  </si>
+  <si>
+    <t>Schiedam</t>
+  </si>
+  <si>
+    <t>update diff layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -771,7 +777,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -779,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>49</v>
       </c>
@@ -1379,12 +1385,22 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>50</v>
       </c>
       <c r="I82" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>